<commit_message>
Fixed mistakes, added use cases, generated reports
</commit_message>
<xml_diff>
--- a/config/belviq cardio adr vs obesity control.xlsx
+++ b/config/belviq cardio adr vs obesity control.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cardio non valve and pulmonary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="105">
   <si>
     <t>Acute myocardial infarction</t>
   </si>
@@ -340,97 +340,7 @@
     <t>Xenical</t>
   </si>
   <si>
-    <t>control A</t>
-  </si>
-  <si>
-    <t>control B</t>
-  </si>
-  <si>
-    <t>Liraglutide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saxenda </t>
-  </si>
-  <si>
-    <t>Naltrexone and bupropion</t>
-  </si>
-  <si>
-    <t>naltrexone hydrochloride and bupropion hydrochloride</t>
-  </si>
-  <si>
-    <t>Contrave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contrave extended-release  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bupropion/Naltrexone</t>
-  </si>
-  <si>
-    <t>Naltrexone/bupropion</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bupropion\Naltrexone</t>
-  </si>
-  <si>
-    <t>Naltrexon\bupropion</t>
-  </si>
-  <si>
-    <t>Mysimba</t>
-  </si>
-  <si>
-    <t>bupropion+Naltrexone</t>
-  </si>
-  <si>
-    <t>Naltrexon+bupropion</t>
-  </si>
-  <si>
-    <t>Phentermine/topiramate</t>
-  </si>
-  <si>
-    <t>phentermine hydrochloride</t>
-  </si>
-  <si>
-    <t>lomaira</t>
-  </si>
-  <si>
-    <t>Suprenza</t>
-  </si>
-  <si>
-    <t>phentermine HCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> phentermine resin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adipex-P</t>
-  </si>
-  <si>
-    <t>Qsymia</t>
-  </si>
-  <si>
-    <t>topiramate/Phentermine</t>
-  </si>
-  <si>
-    <t>Phentermine and topiramate</t>
-  </si>
-  <si>
-    <t>topiramate and Phentermine</t>
-  </si>
-  <si>
-    <t>phentermine</t>
-  </si>
-  <si>
-    <t>topiramate\Phentermine</t>
-  </si>
-  <si>
-    <t>topiramate+Phentermine</t>
-  </si>
-  <si>
-    <t>Phentermine\topiramate</t>
-  </si>
-  <si>
-    <t>Phentermine+topiramate</t>
+    <t xml:space="preserve">control </t>
   </si>
 </sst>
 </file>
@@ -783,20 +693,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="C1:D32"/>
+    <sheetView rightToLeft="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="45.875" customWidth="1"/>
-    <col min="3" max="3" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -806,11 +715,8 @@
       <c r="C1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -820,11 +726,8 @@
       <c r="C2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -834,243 +737,153 @@
       <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
@@ -1294,20 +1107,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.25" customWidth="1"/>
-    <col min="3" max="3" width="24.25" customWidth="1"/>
-    <col min="4" max="4" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1317,11 +1129,8 @@
       <c r="C1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -1331,11 +1140,8 @@
       <c r="C2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1345,231 +1151,133 @@
       <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1585,20 +1293,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1608,594 +1315,529 @@
       <c r="C1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    </row>
+    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="28" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>32</v>
-      </c>
-      <c r="C28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>44</v>
+      <c r="B40" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="55" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="57" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="58" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="59" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="60" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
+    <row r="61" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
+    <row r="62" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
+    <row r="63" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
+    <row r="64" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>75</v>
+      <c r="B69" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B80" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="5" t="s">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B87" s="5" t="s">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B90" s="2" t="s">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10030001"/>
-    <hyperlink ref="B9" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10011108"/>
-    <hyperlink ref="B10" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10021922"/>
-    <hyperlink ref="B20" r:id="rId4" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078240"/>
-    <hyperlink ref="B21" r:id="rId5" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036886"/>
-    <hyperlink ref="B23" r:id="rId6" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10037705"/>
-    <hyperlink ref="B24" r:id="rId7" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078242"/>
-    <hyperlink ref="B26" r:id="rId8" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10003674"/>
-    <hyperlink ref="B27" r:id="rId9" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10054581"/>
-    <hyperlink ref="B34" r:id="rId10" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014387"/>
-    <hyperlink ref="B59" r:id="rId11" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10043821"/>
-    <hyperlink ref="B60" r:id="rId12" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036359"/>
-    <hyperlink ref="B62" r:id="rId13" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10023027"/>
-    <hyperlink ref="B63" r:id="rId14" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014515"/>
-    <hyperlink ref="B65" r:id="rId15" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10072761"/>
-    <hyperlink ref="B66" r:id="rId16" display="http://bioportal.bioontology.org/ontologies/ICD10?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10%2FI05.9"/>
-    <hyperlink ref="B72" r:id="rId17" display="http://bioportal.bioontology.org/ontologies/CRISP?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FCSP%2F1393-3777"/>
-    <hyperlink ref="B74" r:id="rId18" display="http://bioportal.bioontology.org/ontologies/SNOMEDCT?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FSNOMEDCT%2F194732001"/>
-    <hyperlink ref="B90" r:id="rId19" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10026985"/>
+    <hyperlink ref="B4" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10CM?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10CM%2FI21.3"/>
+    <hyperlink ref="B14" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10030001"/>
+    <hyperlink ref="B15" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10011108"/>
+    <hyperlink ref="B16" r:id="rId4" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10021922"/>
+    <hyperlink ref="B26" r:id="rId5" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078240"/>
+    <hyperlink ref="B27" r:id="rId6" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036886"/>
+    <hyperlink ref="B29" r:id="rId7" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10037705"/>
+    <hyperlink ref="B30" r:id="rId8" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078242"/>
+    <hyperlink ref="B32" r:id="rId9" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10003674"/>
+    <hyperlink ref="B33" r:id="rId10" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10054581"/>
+    <hyperlink ref="B40" r:id="rId11" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014387"/>
+    <hyperlink ref="B65" r:id="rId12" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10043821"/>
+    <hyperlink ref="B66" r:id="rId13" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036359"/>
+    <hyperlink ref="B68" r:id="rId14" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10023027"/>
+    <hyperlink ref="B69" r:id="rId15" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014515"/>
+    <hyperlink ref="B71" r:id="rId16" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10072761"/>
+    <hyperlink ref="B72" r:id="rId17" display="http://bioportal.bioontology.org/ontologies/ICD10?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10%2FI05.9"/>
+    <hyperlink ref="B78" r:id="rId18" display="http://bioportal.bioontology.org/ontologies/CRISP?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FCSP%2F1393-3777"/>
+    <hyperlink ref="B80" r:id="rId19" display="http://bioportal.bioontology.org/ontologies/SNOMEDCT?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FSNOMEDCT%2F194732001"/>
+    <hyperlink ref="B96" r:id="rId20" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10026985"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>